<commit_message>
Form Page and screenshot
09/29/2021
</commit_message>
<xml_diff>
--- a/seleniums/src/main/java/testData/TestData.xlsx
+++ b/seleniums/src/main/java/testData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_3a1\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3ADD6DE-EFD8-468C-9F69-BF02C0AB94FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C93CEF0-9F12-4BBF-B43D-9FEF27586230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Id</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>ID02</t>
   </si>
 </sst>
 </file>
@@ -945,10 +948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1029,9 +1032,45 @@
         <v>8019271171</v>
       </c>
     </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="2">
+        <v>50037</v>
+      </c>
+      <c r="K3" s="2">
+        <v>8019271171</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{2D70334F-DE08-4513-81C4-EF75F9310C10}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{8DEE5C39-436D-4677-AC4B-7FCE0D034436}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>